<commit_message>
Code submitted on 16July from office
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF6C243-9636-4B56-9867-0670CA9C1739}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B3C13-9309-48AD-A0EC-062BDEAB84D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="5925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,73 +43,55 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>06/24/2019</t>
-  </si>
-  <si>
-    <t>06/25/2019</t>
-  </si>
-  <si>
-    <t>06/26/2019</t>
-  </si>
-  <si>
-    <t>06/27/2019</t>
-  </si>
-  <si>
-    <t>06/28/2019</t>
-  </si>
-  <si>
-    <t>1.	Created below defects as per observations discussed yesterday:
-#7840: The thick dividing line is not appearing above the section “Your 2018 orders”. Also, the date format is not as per the mock-up.
-#7841: Colon ":" is not suffixed along the headers on page "ChangeOrderList.aspx" and "CustomerAddress.aspx"
-#7842:Layout on the page "ChangeOrderList.aspx" is still showing as the older one if there are no recent orders for the logged in user.
-#7843:Buttons are not centered with the text fields on both sections on CustomerProfile.aspx page
-2.	Updated/Added test cases for #6791: Mobile round corner block refresh.
-3.	Verified changes on more pages under ticket : #6791: Mobile round corner block refresh. Please find attached the list of pages tested as part of #6791(with or without mockups) along with the list of pages that are not in scope of QA for now. Also, mentioned the changes tested on pages for which mock-ups are not available. Please review the list and confirm the scope. Also, sent a separate email for this. Observations raised today can be found at: https://pmall4-my.sharepoint.com/:w:/g/personal/neerajv_pmall_com/EUF91xWaip1Bu09EbHpD5xQBBtKNdHpi14Uo3Nnq29ZwFw?e=669UV6
-4.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.</t>
-  </si>
-  <si>
-    <t>1.	Created Defect #7832: Catalog sale price is not getting displayed under products on Branding Page, in PMall admin.
-2.	Updated/Added test cases for #6791: Mobile round corner block refresh.
-3.	Verified changes on more pages under ticket : #6791: Mobile round corner block refresh. Will create defects as per the discussed observations along with other updates in PMall admin, tomorrow.
-4.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.
-5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
-  </si>
-  <si>
-    <t>1.	Created below defects as per observations discussed yesterday:
-#7815: Customer ratings are not getting displayed under products on Greeting Cards PopUp Window, although the ratings are present for the product on the product page
-#7817: Sdest id is not correct in query string of products on Greeting Cards pop up window on checkout page.  
-#7818: Image size of Products is not correct on Product Brand Group pages on mobile. The size of circular color swatch is also not correct.
-#7819: The alignment of the text in paragraph under the Brand logo on Product Brand Group page is not correct on mobile
-#7820: Image size of products and size of color swatch under products is not correct on collection pages on mobile.
-#7823: Catalog Price is not getting displayed under products on Greeting Cards pop up window.
-2.	Retested defect #7748. This defect failed retest. Please refer attached screenshots in PMall admin.
-3.	Verified remaining scenarios for project #7303:Gift Options at Checkout and updated results.
-4.	Verified the changes for four pages under My Accounts section so far made as part of project #6791: Mobile round corner block refresh. Please find the observations found at: https://pmall4-my.sharepoint.com/:w:/g/personal/neerajv_pmall_com/EZEJOFRWtDNEuaA92i08Gz8BttBan53cnu9sD_MoQb2MvA?e=cu0HNG
-5.	Verified defect 7783 in browser stack as well. It is reproducible in browser stack too. Updated comments in the ticket in PMall admin.
-6.	Updated/Added test cases for #6791: Mobile round corner block refresh and #7303:Gift Options at Checkout.
-7.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.</t>
-  </si>
-  <si>
-    <t>1.	Created below defects as per observations discussed yesterday:
-•	#7801: Alt text missing on the brand logo images on Product Brand Group page(with or without Artist name)
-•	#7802: Only the product name is clickable in the products shown on Product Group brand page on mobile and not the image or any other element in the entire product block.
-•	#7803: On mobile site map, clicking on any of the headers "Product Design Collections, Product Brand Collections and Gift Guides", user is navigated to "Personalized-Gifts-Product-Categories-z3.store"
-•	#7804: Alt text is missing on images on product page.
-•	#7805: 404 error is getting displayed for two images on searching the product "21668-2" or after adding the product to cart.
-2.	Retested defects #7782(Pass) and #7783(Rejected). Added screenshots in PMall admin .
-3.	Verified issue #7809. Not able to reproduce it on either mobile or Desktop. Shared details in another email. Still watching the issue.
-4.	Performed remaining test execution on #7539: Brand logo &amp; Artist Page on mobile site. Will create defects as per discussed observations tomorrow.
-5.	Verified changes deployed for #7303:Gift Options at Checkout section on checkout page. Will create defects as per discussed observations tomorrow.
-6.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.
-7.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
-  </si>
-  <si>
-    <t>1.	Performed high level verification of below changes deployed today. Dev environment was down during the day today. Ticket #7303 is blocked for testing due to an issue reported on another email.
-•	#6791: Mobile round corner block refresh
-•	#7303: Gift Options at Checkout
-2.	Shared the list of pages under My Accounts on which major changes are visible as part of project #6791 on another email. Kindly , confirm the scope for this project.
-3.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.
-4.	Attended daily status meeting to discuss project updates, tasks , observations and requirements. Will create defects in PMall admin as per observations discussed today.</t>
+    <t>07/08/2019</t>
+  </si>
+  <si>
+    <t>07/09/2019</t>
+  </si>
+  <si>
+    <t>07/10/2019</t>
+  </si>
+  <si>
+    <t>07/11/2019</t>
+  </si>
+  <si>
+    <t>07/12/2019</t>
+  </si>
+  <si>
+    <t>1.	Created defect #7907 for the production issue(Access Denied on CreateProfile.aspx page). Tried to reproduce the issue in different ways, but not able to reproduce it here. Please refer the mail sent for details.
+2.	Created defect #7908 as per yesterday’s observations shared with Sonny and assigned it to him in PMall admin.
+3.	Worked on creation of Life Cycle for a Project/Feature/Defect in PMall admin. Shared the initial draft in separate email. Please review and suggest.
+4.	Tried to reproduce the other production issue reported yesterday for iPad, but not able to reproduce that too. Please refer the email shared for more details. Also, attached the same here for reference.
+5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
+6.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.</t>
+  </si>
+  <si>
+    <t>1.	Retested defect #7746 again on dev environment which is failing retest on dev as well for issue 2. Assigned it to you for review. Please review and suggest.
+2.	Created defects #7900, #7901, #7902 in PMall admin as per Sonny’s response on yesterday’s observations.
+3.	Retested defects #7815 and #7817. Please respond on query shared regarding defect #7817.
+4.	Verified “Re-order This Item” functionality from Order Details page on mobile site as part of #6791. Shared observations with Sonny for review.
+5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
+6.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
+  </si>
+  <si>
+    <t>1.	Performed regression test on live environment on both mobile and desktop site. No issues found. Shared status in a separate email.
+2.	Retested defect #7746 on dev environment which is failing retest. Assigned it back to Sonny for review. Will update the same as per our discussion in today’s stand-up call.
+3.	Verified 3 new pages as part of #6791 on dev environment. Shared observations with Sonny and you on email. Please review and let me know if defects need to be created against them.
+4.	Reviewed errors appearing in Bug snag tool. Need to discuss the same to identify the priority and where to raise them.
+5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
+6.	Will reschedule daily stand-up call to 11:15 AM(Chicago time), yesterday onwards.
+7.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
+  </si>
+  <si>
+    <t>1.	Retested defects assigned to me in PMall admin. Shared detailed status in a separate email, attached here for reference.
+2.	Created defects #7890 and #7891 based on discussion on yesterday’s observations and assigned them to Sonny.
+3.	Worked on verification of more pages as per Sonny’s confirmation on scope of ticket #6791 - Mobile round corner block refresh. Will share observations if any once complete.
+4.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
+  </si>
+  <si>
+    <t>1.	Performed ad-hoc testing on different tickets deployed on Dev environment as part of June Release.
+2.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.
+3.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
   </si>
 </sst>
 </file>
@@ -556,7 +538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -570,7 +552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="390" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -584,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -598,7 +580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -612,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="345" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Commit on 30 July -office.
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B3C13-9309-48AD-A0EC-062BDEAB84D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3062C8A-7BB6-4396-AF6C-9D7B430BE1A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14880" windowHeight="5925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,55 +44,56 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>07/08/2019</t>
-  </si>
-  <si>
-    <t>07/09/2019</t>
-  </si>
-  <si>
-    <t>07/10/2019</t>
-  </si>
-  <si>
-    <t>07/11/2019</t>
-  </si>
-  <si>
-    <t>07/12/2019</t>
-  </si>
-  <si>
-    <t>1.	Created defect #7907 for the production issue(Access Denied on CreateProfile.aspx page). Tried to reproduce the issue in different ways, but not able to reproduce it here. Please refer the mail sent for details.
-2.	Created defect #7908 as per yesterday’s observations shared with Sonny and assigned it to him in PMall admin.
-3.	Worked on creation of Life Cycle for a Project/Feature/Defect in PMall admin. Shared the initial draft in separate email. Please review and suggest.
-4.	Tried to reproduce the other production issue reported yesterday for iPad, but not able to reproduce that too. Please refer the email shared for more details. Also, attached the same here for reference.
-5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
-6.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date.</t>
-  </si>
-  <si>
-    <t>1.	Retested defect #7746 again on dev environment which is failing retest on dev as well for issue 2. Assigned it to you for review. Please review and suggest.
-2.	Created defects #7900, #7901, #7902 in PMall admin as per Sonny’s response on yesterday’s observations.
-3.	Retested defects #7815 and #7817. Please respond on query shared regarding defect #7817.
-4.	Verified “Re-order This Item” functionality from Order Details page on mobile site as part of #6791. Shared observations with Sonny for review.
-5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
-6.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
-  </si>
-  <si>
-    <t>1.	Performed regression test on live environment on both mobile and desktop site. No issues found. Shared status in a separate email.
-2.	Retested defect #7746 on dev environment which is failing retest. Assigned it back to Sonny for review. Will update the same as per our discussion in today’s stand-up call.
-3.	Verified 3 new pages as part of #6791 on dev environment. Shared observations with Sonny and you on email. Please review and let me know if defects need to be created against them.
-4.	Reviewed errors appearing in Bug snag tool. Need to discuss the same to identify the priority and where to raise them.
-5.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.
-6.	Will reschedule daily stand-up call to 11:15 AM(Chicago time), yesterday onwards.
-7.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
-  </si>
-  <si>
-    <t>1.	Retested defects assigned to me in PMall admin. Shared detailed status in a separate email, attached here for reference.
-2.	Created defects #7890 and #7891 based on discussion on yesterday’s observations and assigned them to Sonny.
-3.	Worked on verification of more pages as per Sonny’s confirmation on scope of ticket #6791 - Mobile round corner block refresh. Will share observations if any once complete.
-4.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.</t>
-  </si>
-  <si>
-    <t>1.	Performed ad-hoc testing on different tickets deployed on Dev environment as part of June Release.
-2.	Updated testing status report for June release. Please find attached sheet with updated Ticket-Wise Test Summary, Test Case Execution Summary, Test cases and Defects created in June release till date. Also shared detailed status in a separate email.
-3.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
+    <t>07/22/2019</t>
+  </si>
+  <si>
+    <t>07/23/2019</t>
+  </si>
+  <si>
+    <t>07/24/2019</t>
+  </si>
+  <si>
+    <t>07/25/2019</t>
+  </si>
+  <si>
+    <t>07/26/2019</t>
+  </si>
+  <si>
+    <t>1.	Performed functional testing for remaining tickets today on Chrome Browser on Dev environment. Testing is pending for all tickets on different browsers and devices. Testing for #7539: Brand logo &amp; Artist Page is on hold for now as per yesterday’s discussion.
+•	#7304: Mobile Checkout Progress Bar
+•	#7571: Product Page Thumbnail Image Enhancement
+•	#7645: Mobile strike through fix
+•	#6380 : #Add 301 Redirects
+•	#7383: Wedding Page Refresh with new Template
+•	#6791: Mobile round corner block refresh
+2.	Reviewed BugSnag errors for both mobile and desktop.
+3.	Retested defects #7908, #7843 and #7891 on dev environment.
+4.	Attended daily status meeting to discuss all observations found today and yesterday. Created 19 new defects from #7994 – #8012 including the bug snag errors and other console errors discussed today.
+5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
+  </si>
+  <si>
+    <t>1.	Retested  defect #7734 on dev environment assigned to me in PMall admin. Working fine on dev environment.
+2.	Completed task # 4410: Implement Facebook DPA Tags in PMall admin.
+3.	Performed testing on Gift Checkout Options on both mobile and desktop site on chrome browser. Shared observation documents with you and other developers on a separate email.
+4.	Created 7 new defects from #7980 to #7986.
+5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
+  </si>
+  <si>
+    <t>1.	Retested defects assigned to me in PMall admin: #7890, #7803, #7817, #7652 and #6990.
+2.	Performed further testing on #7799: Website logo update and #7539: Brand logo &amp; Artist Page. Multiple issues are appearing on the branding page as discussed in call. I will discontinue testing on the same until further intimation.
+3.	Attended daily standup. Discussed observations raised on 23rd July along with other issues. Mailed all issues to Sonny and Vinod on separate emails. Will verify the same tomorrow and raise the defects in PMall admin if any of them persist. Also, had discussion with Vinod for the scope of #7873.
+4.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.	Verified the new functionalities on dev environment: #7799: Website Logo Update(desktop and mobile site) and #7873:Desktop Product Category Featured Redirected Store/Category Items. Shared observations with you and dev team for review.
+2.	Created/Updated test cases for #7799 and #7873.
+3.	Created status report for June release-cycle 2 which includes most of the tickets tested previously that are to be regressed or retested because of new changes, along with some new tickets deployed in July. Please find attached updated status report with Ticket-Wise Test Summary- Cycle 2, Test Case Execution Summary- Cycle 2, Test cases and Defects created in June release till date. </t>
+  </si>
+  <si>
+    <t>1.	Reviewed Bug Snag errors for both PMall mobile and desktop site for dev environment. Created 3 new defects and assigned to Vinod for review.
+2.	Verified the ticket #7950 and shared a minor observation with you on email. Kindly review and suggest.
+3.	Observed large number of errors appearing in browser console for both desktop and mobile site. Shared screenshots in another email. Please review and suggest.
+4.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -566,7 +568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -580,7 +582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -594,7 +596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Latest Commit on 20August from office
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3062C8A-7BB6-4396-AF6C-9D7B430BE1A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD52CEB-20B5-4C97-BEE3-3FE80C3138E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -44,56 +44,14 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>07/22/2019</t>
-  </si>
-  <si>
-    <t>07/23/2019</t>
-  </si>
-  <si>
-    <t>07/24/2019</t>
-  </si>
-  <si>
-    <t>07/25/2019</t>
-  </si>
-  <si>
-    <t>07/26/2019</t>
-  </si>
-  <si>
-    <t>1.	Performed functional testing for remaining tickets today on Chrome Browser on Dev environment. Testing is pending for all tickets on different browsers and devices. Testing for #7539: Brand logo &amp; Artist Page is on hold for now as per yesterday’s discussion.
-•	#7304: Mobile Checkout Progress Bar
-•	#7571: Product Page Thumbnail Image Enhancement
-•	#7645: Mobile strike through fix
-•	#6380 : #Add 301 Redirects
-•	#7383: Wedding Page Refresh with new Template
-•	#6791: Mobile round corner block refresh
-2.	Reviewed BugSnag errors for both mobile and desktop.
-3.	Retested defects #7908, #7843 and #7891 on dev environment.
-4.	Attended daily status meeting to discuss all observations found today and yesterday. Created 19 new defects from #7994 – #8012 including the bug snag errors and other console errors discussed today.
+    <t>1.	Verified Branding page on Desktop and Mobile site. Testing is blocked for now due to some new pages showing under site map, updated just some time before, which have lots of issues. Please restore the pages to stable ones for further testing. 
+2.	Identified some console errors in the application. Please find observations along with console errors in the document at: https://pmall4-my.sharepoint.com/:w:/g/personal/neerajv_pmall_com/ESEBSFeusalLj3EIWOfvezgB0imt1neXQp_iwQg7PB517Q?e=OhBA5z
+3.	Created 3 defects: #8015, #8016 and #8017 on dev environment.
+4.	Retested defect #7732 on dev environment. Working fine on dev.
 5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
   </si>
   <si>
-    <t>1.	Retested  defect #7734 on dev environment assigned to me in PMall admin. Working fine on dev environment.
-2.	Completed task # 4410: Implement Facebook DPA Tags in PMall admin.
-3.	Performed testing on Gift Checkout Options on both mobile and desktop site on chrome browser. Shared observation documents with you and other developers on a separate email.
-4.	Created 7 new defects from #7980 to #7986.
-5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
-  </si>
-  <si>
-    <t>1.	Retested defects assigned to me in PMall admin: #7890, #7803, #7817, #7652 and #6990.
-2.	Performed further testing on #7799: Website logo update and #7539: Brand logo &amp; Artist Page. Multiple issues are appearing on the branding page as discussed in call. I will discontinue testing on the same until further intimation.
-3.	Attended daily standup. Discussed observations raised on 23rd July along with other issues. Mailed all issues to Sonny and Vinod on separate emails. Will verify the same tomorrow and raise the defects in PMall admin if any of them persist. Also, had discussion with Vinod for the scope of #7873.
-4.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.	Verified the new functionalities on dev environment: #7799: Website Logo Update(desktop and mobile site) and #7873:Desktop Product Category Featured Redirected Store/Category Items. Shared observations with you and dev team for review.
-2.	Created/Updated test cases for #7799 and #7873.
-3.	Created status report for June release-cycle 2 which includes most of the tickets tested previously that are to be regressed or retested because of new changes, along with some new tickets deployed in July. Please find attached updated status report with Ticket-Wise Test Summary- Cycle 2, Test Case Execution Summary- Cycle 2, Test cases and Defects created in June release till date. </t>
-  </si>
-  <si>
-    <t>1.	Reviewed Bug Snag errors for both PMall mobile and desktop site for dev environment. Created 3 new defects and assigned to Vinod for review.
-2.	Verified the ticket #7950 and shared a minor observation with you on email. Kindly review and suggest.
-3.	Observed large number of errors appearing in browser console for both desktop and mobile site. Shared screenshots in another email. Please review and suggest.
-4.	Attended daily status meeting to discuss project updates, tasks , observations and requirements.</t>
+    <t>08/16/2019</t>
   </si>
 </sst>
 </file>
@@ -513,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -540,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -548,66 +506,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="240" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The master branch copy 1
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD52CEB-20B5-4C97-BEE3-3FE80C3138E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB514919-A55C-4DA2-AF4D-E83410611BB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -44,14 +44,37 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>1.	Verified Branding page on Desktop and Mobile site. Testing is blocked for now due to some new pages showing under site map, updated just some time before, which have lots of issues. Please restore the pages to stable ones for further testing. 
-2.	Identified some console errors in the application. Please find observations along with console errors in the document at: https://pmall4-my.sharepoint.com/:w:/g/personal/neerajv_pmall_com/ESEBSFeusalLj3EIWOfvezgB0imt1neXQp_iwQg7PB517Q?e=OhBA5z
-3.	Created 3 defects: #8015, #8016 and #8017 on dev environment.
-4.	Retested defect #7732 on dev environment. Working fine on dev.
-5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
-  </si>
-  <si>
-    <t>08/16/2019</t>
+    <t>09/09/2019</t>
+  </si>
+  <si>
+    <t>09/10/2019</t>
+  </si>
+  <si>
+    <t>09/11/2019</t>
+  </si>
+  <si>
+    <t>09/12/2019</t>
+  </si>
+  <si>
+    <t>1.	Worked on the test case update and test execution of #6642: Cart page redesign on Chrome browser. Created defects #8269 and #8270 as discussed. Will cancel defect #8269 as per discussion and create another defect from the observations discussed today. Please find updated test report attached.
+2.	The dev preview is not working on dev environment. Shared the issue in a separate email.
+3.	Attended daily stand-up to triage the defects in September release. The defects that are on dev for testing are marked as “On Dev” in smartsheet and highlighted in green. All the other defects that are in scope of September release are marked as “In Progress”  and highlighted in yellow. All the highlighted defects have been at the top under section “Defects” in September release.
+4.	Attended the automation meeting with Noah. Discussed the new updates and queries related to Git and execution of the features ready to run.</t>
+  </si>
+  <si>
+    <t>1.	Added all open defects from August release to September release and consolidated the list under a single “Defects” section. Also, updated the status and developer’s name against all the defects.
+2.	Worked on verification of the functional scenarios on the #6642: Cart page redesign and #8164: Contact us page add Google recaptcha. Also, updated test cases for ticket: #8164. Please find attached updated Test Report for September release.</t>
+  </si>
+  <si>
+    <t>1.	Verified the issue shared by you, with the space along the images appearing under two columns in section “Recommended For You” on mobile site on home page, on different versions of iOS and Android on different screen size and browsers through Browser-Stack. Shared analysis in another email.
+2.	Worked on verification of the functional scenarios on the Cart page on desktop site as part of #6642. Also, updated test cases for ticket: #6642: Cart page redesign. Also, added the tickets deployed and tested last Friday in the September release test report. Please find the updated test report attached.
+3.	Attended daily automation meeting with Noah and discussed queries and other updates.
+4.	Updated the products/items against the regression test cases and shared updated sheet with Noah.
+5.	Attended daily stand up meeting to discuss updates, queries, tasks and requirements.</t>
+  </si>
+  <si>
+    <t>1.	Worked on understanding of the Cucumber Framework elements (Features, Step Definitions, Hooks, Tags and Test Runner), implemented for automation as shown by Noah in our last call.  Also, analyzed the project created by Noah on Dev Server and worked on set- up of IJ IDE and other software’s required for Automation on my local. Set-up is still in progress.
+2.	Attended the automation meeting with Noah and shared the challenges identified after the analyses of the BDD framework, implemented for personalization of the  products , so far. Let’s discuss the same in our daily stand up call tomorrow. Will continue with further analysis of the Automation project and share the feedback with you and Noah.</t>
   </si>
 </sst>
 </file>
@@ -471,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -506,10 +529,52 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first commit on 24 October from command line
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB514919-A55C-4DA2-AF4D-E83410611BB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9268B3AF-0377-4BF8-86A0-FDA979AD33A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -44,37 +44,58 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>09/09/2019</t>
-  </si>
-  <si>
-    <t>09/10/2019</t>
-  </si>
-  <si>
-    <t>09/11/2019</t>
-  </si>
-  <si>
-    <t>09/12/2019</t>
-  </si>
-  <si>
-    <t>1.	Worked on the test case update and test execution of #6642: Cart page redesign on Chrome browser. Created defects #8269 and #8270 as discussed. Will cancel defect #8269 as per discussion and create another defect from the observations discussed today. Please find updated test report attached.
-2.	The dev preview is not working on dev environment. Shared the issue in a separate email.
-3.	Attended daily stand-up to triage the defects in September release. The defects that are on dev for testing are marked as “On Dev” in smartsheet and highlighted in green. All the other defects that are in scope of September release are marked as “In Progress”  and highlighted in yellow. All the highlighted defects have been at the top under section “Defects” in September release.
-4.	Attended the automation meeting with Noah. Discussed the new updates and queries related to Git and execution of the features ready to run.</t>
-  </si>
-  <si>
-    <t>1.	Added all open defects from August release to September release and consolidated the list under a single “Defects” section. Also, updated the status and developer’s name against all the defects.
-2.	Worked on verification of the functional scenarios on the #6642: Cart page redesign and #8164: Contact us page add Google recaptcha. Also, updated test cases for ticket: #8164. Please find attached updated Test Report for September release.</t>
-  </si>
-  <si>
-    <t>1.	Verified the issue shared by you, with the space along the images appearing under two columns in section “Recommended For You” on mobile site on home page, on different versions of iOS and Android on different screen size and browsers through Browser-Stack. Shared analysis in another email.
-2.	Worked on verification of the functional scenarios on the Cart page on desktop site as part of #6642. Also, updated test cases for ticket: #6642: Cart page redesign. Also, added the tickets deployed and tested last Friday in the September release test report. Please find the updated test report attached.
-3.	Attended daily automation meeting with Noah and discussed queries and other updates.
-4.	Updated the products/items against the regression test cases and shared updated sheet with Noah.
-5.	Attended daily stand up meeting to discuss updates, queries, tasks and requirements.</t>
-  </si>
-  <si>
-    <t>1.	Worked on understanding of the Cucumber Framework elements (Features, Step Definitions, Hooks, Tags and Test Runner), implemented for automation as shown by Noah in our last call.  Also, analyzed the project created by Noah on Dev Server and worked on set- up of IJ IDE and other software’s required for Automation on my local. Set-up is still in progress.
-2.	Attended the automation meeting with Noah and shared the challenges identified after the analyses of the BDD framework, implemented for personalization of the  products , so far. Let’s discuss the same in our daily stand up call tomorrow. Will continue with further analysis of the Automation project and share the feedback with you and Noah.</t>
+    <t>10/14/2019</t>
+  </si>
+  <si>
+    <t>10/15/2019</t>
+  </si>
+  <si>
+    <t>10/16/2019</t>
+  </si>
+  <si>
+    <t>10/17/2019</t>
+  </si>
+  <si>
+    <t>10/18/2019</t>
+  </si>
+  <si>
+    <t>10/21/2019</t>
+  </si>
+  <si>
+    <t>1.	Updated all mobile site scenarios and collaborated them with Desktop ones in the required format in automation test scenarios smartsheet. Added few comments for Noah to update. Please review and suggest.
+2.	Verified few PMall pages using the Varvy  SEO inspector tool as per the assigned ticket #8394. Need to discuss it before moving on what issues to be reported in what format and also about the scope of verification.
+3.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet.
+4.	Reviewed the requirements of the October release tickets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.	Created 3 new defects from #8529 - #8531 in PMall admin and added them to smartsheet as well.
+2.	Closed all the tickets from September release scope as discussed yesterday. Please find the updated September release sheet attached.
+3.	Worked on mobile automation scripts review in smartsheet. Will consolidate scripts with desktop ones and share the updated scripts by Monday.
+4.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet. Also, discussed the daily automation jobs on autoqa2 server. </t>
+  </si>
+  <si>
+    <t>1.	Created 6 new defects from #8517 - #8522 in PMall admin as per observations discussed yesterday. 
+2.	Reviewed automation script code for Desktop site to understand the structure.
+3.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet. Please review the backlog section in the automation scenarios smartsheet and prioritize the scope.
+4.	Attended daily status call. Discussed tickets in September release that need to be closed or moved to October release. Will update the status of tickets in PMall admin as per discussion and update status in smartsheet too, accordingly.</t>
+  </si>
+  <si>
+    <t>1.	Performed cross browser testing on mobile site  on iOS 12 and Android 7 around the September release tickets. No issues found.
+2.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet. Please review the backlog section in the automation scenarios smartsheet and prioritize the scope.
+3.	Discussed All production issues shared on email on 10th  and 11th October. Will create the defects against the reviewed issues in PMall admin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.	Updated the automation test cases in the smartsheet. Discussed some changes with Noah. Will be ready for review, once Noah implement those changes. Also, added a Backlog section in the sheet to consolidate the scope for automation on PMall Website. Please review and provide your feedback. Also, could you please prioritize the backlog items as per the required order of implementation.
+2.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet.
+3.	Verified the ticket #7734 on prod environment. Updated results in PMall admin. Please review.
+4.	Updated Test results in September release smartsheet. Please find updated sheet attached.
+ </t>
+  </si>
+  <si>
+    <t>1.	Updated the automation test cases in the smartsheet. Will share the updated sheet after the discussed changes are implemented by Noah.
+2.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet.
+3.	Reviewed the requirements against Christmas Cards Store Banner [#8496].
+4.	Verified #8398 on mobile and desktop site. Changes are appearing fine now.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -521,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -532,10 +553,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -546,10 +567,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -560,10 +581,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -574,8 +595,66 @@
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commit on master branch directly
</commit_message>
<xml_diff>
--- a/PMallWeb/Resources/Files/Timesheet.xlsx
+++ b/PMallWeb/Resources/Files/Timesheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD52CEB-20B5-4C97-BEE3-3FE80C3138E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5664FCD-A9BB-4B5F-842C-9E7103F9EF4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -44,14 +44,70 @@
     <t>Test Execution/Defect Documentation/Defect Retest/Testing</t>
   </si>
   <si>
-    <t>1.	Verified Branding page on Desktop and Mobile site. Testing is blocked for now due to some new pages showing under site map, updated just some time before, which have lots of issues. Please restore the pages to stable ones for further testing. 
-2.	Identified some console errors in the application. Please find observations along with console errors in the document at: https://pmall4-my.sharepoint.com/:w:/g/personal/neerajv_pmall_com/ESEBSFeusalLj3EIWOfvezgB0imt1neXQp_iwQg7PB517Q?e=OhBA5z
-3.	Created 3 defects: #8015, #8016 and #8017 on dev environment.
-4.	Retested defect #7732 on dev environment. Working fine on dev.
-5.	Updated status report for June release-cycle 2. Please find updated sheet attached.</t>
-  </si>
-  <si>
-    <t>08/16/2019</t>
+    <t>10/21/2019</t>
+  </si>
+  <si>
+    <t>10/22/2019</t>
+  </si>
+  <si>
+    <t>10/23/2019</t>
+  </si>
+  <si>
+    <t>10/24/2019</t>
+  </si>
+  <si>
+    <t>10/25/2019</t>
+  </si>
+  <si>
+    <t>10/29/2019</t>
+  </si>
+  <si>
+    <t>10/30/2019</t>
+  </si>
+  <si>
+    <t>1.	Worked on creation of test cases for October release. Please find attached sheet for October release with test cases and defects created so far.
+2.	Reviewed the automation test code for understanding.
+3.	Please review all defects added to October release.
+4.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.</t>
+  </si>
+  <si>
+    <t>1.	Worked on creation of test cases for October release. Please find attached sheet for October release with test cases and defects created so far.
+2.	Created defect #8572 and added the same to October release defects.
+3.	Please review all defects added to October release.
+4.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.</t>
+  </si>
+  <si>
+    <t>1.	Worked on creation of test cases for October release tickets discussed.
+2.	Reviewed the automation test automation cases added by Noah in smartsheet.
+3.	Please review all defects added to October release.
+4.	Created defect for blank shipping address issue in PMall admin assign d the same to you.
+5.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.</t>
+  </si>
+  <si>
+    <t>1.	Reviewed all defects added to October release. Prioritized and reordered all the defects after review as per my understanding. Also, closed few of them which were working fine but were not assigned to me. However, I have closed them and marked them as Lived in the October release defects in smartsheet.
+2.	Working on  understanding the automation scripts code for desktop and mobile site, further. Not able to pull the code in the existing developer branch as some SSL issue is showing up which has been confirmed by Noah too during the automation meeting on call. 
+3.	Reviewed the mockups and other requirements discussed yesterday which are part of October release.
+4.	Attended daily automation meeting with Noah. 
+5.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.</t>
+  </si>
+  <si>
+    <t>1.	All changes have been incorporated in smart sheet “eCommerce automation” for both Desktop and Mobile site scenarios. Kindly review and suggest.
+2.	Reviewed the Power shell scripts on AutoQA2 server, for scheduling the automation tasks. Also, reviewing the automation scripts code for desktop and mobile site in detail. Not able to pull the code in the existing developer branch as some SSL issue is showing up which has been confirmed by Noah too during the automation meeting on call. 
+3.	Attended daily automation meeting with Noah. 
+4.	Attended daily status meeting to discuss the requirements of October release.
+5.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.</t>
+  </si>
+  <si>
+    <t>1.	Updated Test scenarios for automation in smartsheet “eCommerce automation” for both Desktop and Mobile site scenarios in smartsheet. Please review and suggest. Also, please review the backlog section in the  smartsheet for further task assignment in Automation.
+2.	Reviewed the Power shell scripts on AutoQA2 server, for scheduling the automation tasks. Also, reviewing the automation scripts code for desktop and mobile site in detail. 
+3.	Need to discuss the Varvy SEO Tool tasks, before moving on further, regarding what issues are to be reported in what format and also about the scope of verification.
+4.	Reviewed the requirements of the October release tickets.</t>
+  </si>
+  <si>
+    <t>1.	Updated all mobile site scenarios and collaborated them with Desktop ones in the required format in automation test scenarios smartsheet. Added few comments for Noah to update. Please review and suggest.
+2.	Verified few PMall pages using the Varvy  SEO inspector tool as per the assigned ticket #8394. Need to discuss it before moving on what issues to be reported in what format and also about the scope of verification.
+3.	Attended daily automation discussion meeting with Noah. Discussed the changes made in Automation test cases in smartsheet.
+4.	Reviewed the requirements of the October release tickets.</t>
   </si>
 </sst>
 </file>
@@ -471,9 +527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -498,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -506,10 +564,94 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>